<commit_message>
update unit costs, and coverage of Vit A and CF education
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2016Sept12/subregionSpreadsheets/Barisal.xlsx
+++ b/input_spreadsheets/Bangladesh/2016Sept12/subregionSpreadsheets/Barisal.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12080" yWindow="-21140" windowWidth="19560" windowHeight="20720" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-2500" yWindow="-21140" windowWidth="18960" windowHeight="21140" tabRatio="500" firstSheet="18" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -3207,8 +3207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3255,7 +3255,7 @@
         <v>64</v>
       </c>
       <c r="B3" s="21">
-        <v>0.6</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="C3" s="2">
         <v>0.85</v>
@@ -3278,7 +3278,7 @@
         <v>0.85</v>
       </c>
       <c r="D4" s="21">
-        <v>3.91</v>
+        <v>3.56</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="13"/>
@@ -3295,7 +3295,7 @@
         <v>0.85</v>
       </c>
       <c r="D5" s="21">
-        <v>230.4</v>
+        <v>48</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="13"/>
@@ -3312,7 +3312,7 @@
         <v>0.85</v>
       </c>
       <c r="D6" s="21">
-        <v>3.91</v>
+        <v>3.56</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="13"/>
@@ -4370,7 +4370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>

</xml_diff>